<commit_message>
not ready for checking
</commit_message>
<xml_diff>
--- a/metadata/2022/hwb_metadata_p6_row_names.xlsx
+++ b/metadata/2022/hwb_metadata_p6_row_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scotsconnect-my.sharepoint.com/personal/victoria_dunn_gov_scot/Documents/Git Repos/HWB Rap Project/hwb-census/metadata/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{14EAFD5F-FEC1-4AC8-A479-EB1722C0FE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AB70B50-0023-4CBA-9874-87C2F94CD321}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{14EAFD5F-FEC1-4AC8-A479-EB1722C0FE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{481F304C-EB27-4F48-8D71-172E64133F14}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="-16200" windowWidth="14400" windowHeight="15600" xr2:uid="{08DF662A-F57B-46A7-AE7E-B4B278B79C2B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{08DF662A-F57B-46A7-AE7E-B4B278B79C2B}"/>
   </bookViews>
   <sheets>
     <sheet name="P6" sheetId="1" r:id="rId1"/>
@@ -671,10 +671,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -995,313 +994,316 @@
   <dimension ref="A1:CW17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="E9" sqref="E1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="23.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:101" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:101" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AM1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AP1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AT1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AU1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AV1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AW1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AX1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AY1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BA1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BB1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BC1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BD1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BE1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BF1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BG1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BH1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BI1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BK1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BL1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BM1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BN1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BO1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BP1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BR1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BS1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BT1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BU1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BV1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="BW1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="BX1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="BY1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CA1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CB1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CC1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CD1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CE1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CF1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CG1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CH1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CI1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CK1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CL1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CM1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CN1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CO1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CP1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CR1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CS1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CT1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="CU1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="CV1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="CW1" s="1" t="s">
         <v>182</v>
       </c>
     </row>

</xml_diff>